<commit_message>
menu client side work
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Bake Potato Pizza</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>Lorem ipsum dolor sit amet, consectetur adipisicing elit. Quos nihil cupiditate ut vero alias quaerat inventore molestias vel suscipit explicabo.</t>
+  </si>
+  <si>
+    <t>images/menu/tuscan-grilled.jpg</t>
   </si>
 </sst>
 </file>
@@ -381,38 +384,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="173.85546875" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="173.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="C1" s="2">
         <v>20.5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="C2" s="2">
         <v>10.5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>